<commit_message>
feat: Bổ sung logic lưu đơn vị bán vào bảng san_pham_don_vi khi import Excel
- Chuyển từ ToModel sang ToCollection để xử lý relationship
- Tự động tạo san_pham_don_vi cho đơn vị cơ bản, đơn vị nhập, đơn vị trung gian
- Hỗ trợ thêm 2 đơn vị phụ tùy chọn (don_vi_phu_1, don_vi_phu_2)
- Cập nhật file Excel mẫu với các cột mới và hướng dẫn chi tiết
- Xử lý transaction để đảm bảo data integrity
</commit_message>
<xml_diff>
--- a/product_import_template.xlsx
+++ b/product_import_template.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="San Pham" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Import San Pham" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Huong Dan" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -32,13 +32,9 @@
     </font>
     <font>
       <b val="1"/>
-      <sz val="14"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
@@ -49,12 +45,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="004472C4"/>
         <bgColor rgb="004472C4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00D9E2F3"/>
-        <bgColor rgb="00D9E2F3"/>
       </patternFill>
     </fill>
   </fills>
@@ -76,18 +66,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -453,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,15 +446,24 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="35" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
     <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="18" customWidth="1" min="8" max="8"/>
-    <col width="30" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="15" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="15" customWidth="1" min="11" max="11"/>
+    <col width="15" customWidth="1" min="12" max="12"/>
+    <col width="20" customWidth="1" min="13" max="13"/>
+    <col width="15" customWidth="1" min="14" max="14"/>
+    <col width="15" customWidth="1" min="15" max="15"/>
+    <col width="20" customWidth="1" min="16" max="16"/>
+    <col width="15" customWidth="1" min="17" max="17"/>
+    <col width="30" customWidth="1" min="18" max="18"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -480,7 +474,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>don_vi_ban</t>
+          <t>don_vi_co_ban</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -490,30 +484,75 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>ti_so_chuyen_doi</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>gia_nhap</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>gia_ban</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>gia_ban_le</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>so_luong</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>ti_so_chuyen_doi</t>
-        </is>
-      </c>
       <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>don_vi_trung</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>ti_le_quy_doi_trung</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>gia_ban_trung</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>don_vi_phu_1</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>ti_le_quy_doi_phu_1</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>gia_ban_phu_1</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>don_vi_phu_2</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>ti_le_quy_doi_phu_2</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>gia_ban_phu_2</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>ghi_chu</t>
         </is>
@@ -522,111 +561,262 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Bia Tiger thùng 24 lon</t>
+          <t>Coca Cola</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>Lon</t>
+          <t>lon</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>Thùng</t>
-        </is>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>280000</v>
-      </c>
-      <c r="E2" s="3" t="n">
-        <v>320000</v>
-      </c>
-      <c r="F2" s="3" t="n">
-        <v>14000</v>
-      </c>
-      <c r="G2" s="4" t="n">
+          <t>thùng</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>220000</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>250000</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>12000</v>
+      </c>
+      <c r="H2" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="H2" s="4" t="n">
-        <v>24</v>
-      </c>
       <c r="I2" s="2" t="inlineStr">
         <is>
-          <t>Bia Tiger 330ml</t>
+          <t>lốc</t>
+        </is>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>65000</v>
+      </c>
+      <c r="L2" s="2" t="inlineStr"/>
+      <c r="M2" s="2" t="inlineStr"/>
+      <c r="N2" s="2" t="inlineStr"/>
+      <c r="O2" s="2" t="inlineStr"/>
+      <c r="P2" s="2" t="inlineStr"/>
+      <c r="Q2" s="2" t="inlineStr"/>
+      <c r="R2" s="2" t="inlineStr">
+        <is>
+          <t>Bia Coca-Cola 330ml</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Coca Cola lốc 6 lon</t>
+          <t>Pepsi</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>Lon</t>
+          <t>lon</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>Lốc</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>50000</v>
-      </c>
-      <c r="E3" s="3" t="n">
+          <t>thùng</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>200000</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>240000</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>11000</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="I3" s="2" t="inlineStr">
+        <is>
+          <t>lốc</t>
+        </is>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="K3" s="2" t="n">
         <v>60000</v>
       </c>
-      <c r="F3" s="3" t="n">
-        <v>11000</v>
-      </c>
-      <c r="G3" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="H3" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="I3" s="2" t="inlineStr">
-        <is>
-          <t>Coca 330ml</t>
+      <c r="L3" s="2" t="inlineStr"/>
+      <c r="M3" s="2" t="inlineStr"/>
+      <c r="N3" s="2" t="inlineStr"/>
+      <c r="O3" s="2" t="inlineStr"/>
+      <c r="P3" s="2" t="inlineStr"/>
+      <c r="Q3" s="2" t="inlineStr"/>
+      <c r="R3" s="2" t="inlineStr">
+        <is>
+          <t>Pepsi 330ml</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Mì Hảo Hảo thùng 30 gói</t>
+          <t>Mì Hảo Hảo</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>Gói</t>
+          <t>gói</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>Thùng</t>
-        </is>
-      </c>
-      <c r="D4" s="3" t="n">
+          <t>thùng</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="n">
         <v>90000</v>
       </c>
-      <c r="E4" s="3" t="n">
-        <v>110000</v>
-      </c>
-      <c r="F4" s="3" t="n">
-        <v>4000</v>
-      </c>
-      <c r="G4" s="4" t="n">
-        <v>15</v>
-      </c>
-      <c r="H4" s="4" t="n">
-        <v>30</v>
+      <c r="F4" s="2" t="n">
+        <v>120000</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>4500</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>20</v>
       </c>
       <c r="I4" s="2" t="inlineStr">
         <is>
-          <t>Mì tôm chua cay</t>
+          <t>lốc</t>
+        </is>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="L4" s="2" t="inlineStr"/>
+      <c r="M4" s="2" t="inlineStr"/>
+      <c r="N4" s="2" t="inlineStr"/>
+      <c r="O4" s="2" t="inlineStr"/>
+      <c r="P4" s="2" t="inlineStr"/>
+      <c r="Q4" s="2" t="inlineStr"/>
+      <c r="R4" s="2" t="inlineStr">
+        <is>
+          <t>Mì Hảo Hảo gói 75g</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Dầu ăn Neptune</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>chai</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>thùng</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>300000</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>360000</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>65000</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I5" s="2" t="inlineStr"/>
+      <c r="J5" s="2" t="inlineStr"/>
+      <c r="K5" s="2" t="inlineStr"/>
+      <c r="L5" s="2" t="inlineStr"/>
+      <c r="M5" s="2" t="inlineStr"/>
+      <c r="N5" s="2" t="inlineStr"/>
+      <c r="O5" s="2" t="inlineStr"/>
+      <c r="P5" s="2" t="inlineStr"/>
+      <c r="Q5" s="2" t="inlineStr"/>
+      <c r="R5" s="2" t="inlineStr">
+        <is>
+          <t>Dầu Neptune 1L</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Sữa TH True Milk</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>hộp</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>thùng</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>650000</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>750000</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>17000</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="I6" s="2" t="inlineStr">
+        <is>
+          <t>lốc</t>
+        </is>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>62000</v>
+      </c>
+      <c r="L6" s="2" t="inlineStr"/>
+      <c r="M6" s="2" t="inlineStr"/>
+      <c r="N6" s="2" t="inlineStr"/>
+      <c r="O6" s="2" t="inlineStr"/>
+      <c r="P6" s="2" t="inlineStr"/>
+      <c r="Q6" s="2" t="inlineStr"/>
+      <c r="R6" s="2" t="inlineStr">
+        <is>
+          <t>Sữa TH 180ml</t>
         </is>
       </c>
     </row>
@@ -641,7 +831,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:A33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -649,14 +839,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="45" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="80" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>HƯỚNG DẪN IMPORT SẢN PHẨM</t>
         </is>
@@ -666,260 +853,188 @@
       <c r="A2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="inlineStr">
-        <is>
-          <t>Cột</t>
-        </is>
-      </c>
-      <c r="B3" s="6" t="inlineStr">
-        <is>
-          <t>Mô tả</t>
-        </is>
-      </c>
-      <c r="C3" s="6" t="inlineStr">
-        <is>
-          <t>Bắt buộc</t>
-        </is>
-      </c>
-      <c r="D3" s="6" t="inlineStr">
-        <is>
-          <t>Ví dụ</t>
-        </is>
+      <c r="A3" s="3">
+        <f>== CÁC CỘT BẮT BUỘC ===</f>
+        <v/>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ten_san_pham</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Tên sản phẩm</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Có</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Bia Tiger thùng 24 lon</t>
+          <t>ten_san_pham: Tên sản phẩm (bắt buộc)</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>don_vi_ban</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Đơn vị bán lẻ (đơn vị nhỏ nhất)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Không</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Lon, Chai, Gói, Cái</t>
-        </is>
-      </c>
+      <c r="A5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>don_vi_nhap</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Đơn vị nhập hàng (đơn vị lớn)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Không</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Thùng, Lốc, Bịch, Hộp</t>
-        </is>
+      <c r="A6" s="3">
+        <f>== ĐƠN VỊ TÍNH ===</f>
+        <v/>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>gia_nhap</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Giá nhập (theo đơn vị nhập)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Không</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>280000</t>
+          <t>don_vi_co_ban: Đơn vị nhỏ nhất để bán lẻ (VD: lon, gói, chai, hộp)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>gia_ban</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Giá bán sỉ (theo đơn vị nhập)</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Không</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>320000</t>
+          <t>don_vi_nhap: Đơn vị lớn để nhập hàng (VD: thùng, bao, can)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>gia_ban_le</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Giá bán lẻ (theo đơn vị bán)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Không</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>14000</t>
+          <t>ti_so_chuyen_doi: Số đơn vị cơ bản trong 1 đơn vị nhập (VD: 24 lon = 1 thùng thì nhập 24)</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>so_luong</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Số lượng tồn kho (theo đơn vị nhập)</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Không</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
+      <c r="A10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>ti_so_chuyen_doi</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Số đơn vị bán trong 1 đơn vị nhập</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Không</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>24 (1 thùng = 24 lon)</t>
-        </is>
+      <c r="A11" s="3">
+        <f>== GIÁ CẢ ===</f>
+        <v/>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ghi_chu</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Ghi chú thêm</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Không</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Bia Tiger 330ml</t>
+          <t>gia_nhap: Giá nhập theo đơn vị nhập (VD: giá nhập 1 thùng)</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr"/>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>gia_ban: Giá bán theo đơn vị nhập (VD: giá bán 1 thùng)</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CHÚ Ý:</t>
+          <t>gia_ban_le: Giá bán lẻ theo đơn vị cơ bản (VD: giá bán 1 lon)</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>- Dòng 1 của file phải là header (tên cột)</t>
-        </is>
-      </c>
+      <c r="A15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>- Đơn vị bán và đơn vị nhập có thể nhập tên mới, hệ thống sẽ tự tạo nếu chưa có</t>
-        </is>
+      <c r="A16" s="3">
+        <f>== ĐƠN VỊ TRUNG GIAN (tùy chọn) ===</f>
+        <v/>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>- Giá tiền có thể nhập có hoặc không có dấu phẩy (VD: 280000 hoặc 280,000)</t>
+          <t>don_vi_trung: Đơn vị trung gian (VD: lốc 6 lon)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>- Tỉ số chuyển đổi: VD nhập 24 nghĩa là 1 thùng = 24 lon</t>
+          <t>ti_le_quy_doi_trung: Số đơn vị cơ bản trong 1 đơn vị trung (VD: 6 lon = 1 lốc thì nhập 6)</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>gia_ban_trung: Giá bán theo đơn vị trung</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="3">
+        <f>== ĐƠN VỊ PHỤ 1, 2 (tùy chọn) ===</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Dùng cho các đơn vị bán đặc biệt khác</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="3">
+        <f>== VÍ DỤ ===</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Sản phẩm: Coca Cola</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>- Đơn vị cơ bản: lon (giá bán lẻ 12,000đ)</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>- Đơn vị nhập: thùng 24 lon (giá nhập 220,000đ, giá bán 250,000đ)</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>- Đơn vị trung: lốc 6 lon (giá bán 65,000đ)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="3">
+        <f>== LƯU Ý ===</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>- Số tiền nhập không cần dấu phẩy hoặc chữ 'đ'</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>- Nếu đơn vị chưa có trong hệ thống sẽ tự động tạo mới</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>- Dữ liệu sẽ được lưu vào cả bảng san_pham và san_pham_don_vi</t>
         </is>
       </c>
     </row>

</xml_diff>